<commit_message>
Bugfixes in VPC plots and response on last review
</commit_message>
<xml_diff>
--- a/test/test_NO3/prepareInput/Workflow.xlsx
+++ b/test/test_NO3/prepareInput/Workflow.xlsx
@@ -179,9 +179,6 @@
     <t>sensitivity analysis is performed</t>
   </si>
   <si>
-    <t>Workflow.xlsx</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>xlssheet for sensitivity Parameter definition; if empty first sheet is taken</t>
+  </si>
+  <si>
+    <t>myCalculatePKParameterForApplicationProtocol</t>
   </si>
 </sst>
 </file>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -930,9 +930,6 @@
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -942,7 +939,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
@@ -951,6 +948,9 @@
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
     <row r="22" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1015,10 +1015,10 @@
     </row>
     <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1053,7 +1053,7 @@
         <v>45</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1122,27 +1122,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,27 +1150,27 @@
         <v>12</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
@@ -1178,219 +1178,219 @@
         <v>40</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
         <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
         <v>89</v>
       </c>
-      <c r="C19" t="s">
-        <v>90</v>
-      </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s">
-        <v>92</v>
-      </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bugfixes in VPC plots and response on last review (#20)
</commit_message>
<xml_diff>
--- a/test/test_NO3/prepareInput/Workflow.xlsx
+++ b/test/test_NO3/prepareInput/Workflow.xlsx
@@ -179,9 +179,6 @@
     <t>sensitivity analysis is performed</t>
   </si>
   <si>
-    <t>Workflow.xlsx</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>xlssheet for sensitivity Parameter definition; if empty first sheet is taken</t>
+  </si>
+  <si>
+    <t>myCalculatePKParameterForApplicationProtocol</t>
   </si>
 </sst>
 </file>
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
         <v>13</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -859,7 +859,7 @@
         <v>17</v>
       </c>
       <c r="C7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
@@ -899,7 +899,7 @@
         <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -930,9 +930,6 @@
       <c r="B14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="15" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
@@ -942,7 +939,7 @@
         <v>32</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="39.6" x14ac:dyDescent="0.25">
@@ -951,6 +948,9 @@
       </c>
       <c r="B16" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="C16" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1006,7 +1006,7 @@
     <row r="22" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -1015,10 +1015,10 @@
     </row>
     <row r="23" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
@@ -1026,10 +1026,10 @@
     </row>
     <row r="24" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>101</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>102</v>
       </c>
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
@@ -1053,7 +1053,7 @@
         <v>45</v>
       </c>
       <c r="C26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
@@ -1122,27 +1122,27 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="C2" t="s">
-        <v>59</v>
-      </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1150,27 +1150,27 @@
         <v>12</v>
       </c>
       <c r="B3" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
@@ -1178,219 +1178,219 @@
         <v>40</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C6" t="s">
         <v>67</v>
       </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>
       <c r="B7" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
         <v>70</v>
       </c>
-      <c r="B8" t="s">
-        <v>71</v>
-      </c>
       <c r="C8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B9" t="s">
+        <v>71</v>
+      </c>
+      <c r="C9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D9" t="s">
         <v>72</v>
-      </c>
-      <c r="C9" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
         <v>74</v>
       </c>
-      <c r="C10" t="s">
-        <v>75</v>
-      </c>
       <c r="D10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B11" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
         <v>89</v>
       </c>
-      <c r="C19" t="s">
-        <v>90</v>
-      </c>
       <c r="D19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" t="s">
         <v>91</v>
       </c>
-      <c r="C20" t="s">
-        <v>92</v>
-      </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>